<commit_message>
Updated to include parts for Blinker Circuit.
</commit_message>
<xml_diff>
--- a/Expenses/PCB connector Bill.xlsx
+++ b/Expenses/PCB connector Bill.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/7amoodi/Desktop/Uni/My supermilage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\SVN\trunk\Expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14556" tabRatio="311"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Item #</t>
   </si>
@@ -66,6 +66,57 @@
   </si>
   <si>
     <t>CAD</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>8-DIP Socket for 555</t>
+  </si>
+  <si>
+    <t>A08-LC-TT</t>
+  </si>
+  <si>
+    <t>555 Timer Circuit</t>
+  </si>
+  <si>
+    <t>LM555CN</t>
+  </si>
+  <si>
+    <t>5V Voltage Regulator</t>
+  </si>
+  <si>
+    <t>L7805ABD2T-TR</t>
+  </si>
+  <si>
+    <t>TMK316F106ZL-T</t>
+  </si>
+  <si>
+    <t>10uF Capacitor</t>
+  </si>
+  <si>
+    <t>10nF Capacitor</t>
+  </si>
+  <si>
+    <t>CC1206KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>ERJ-14YJ102U</t>
+  </si>
+  <si>
+    <t>ERJ-14YJ223U</t>
+  </si>
+  <si>
+    <t>22k Resistor</t>
+  </si>
+  <si>
+    <t>50k Resistor</t>
+  </si>
+  <si>
+    <t>CRCW121049K9FKEA</t>
   </si>
 </sst>
 </file>
@@ -130,13 +181,16 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0">
-  <autoFilter ref="A1:G4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G13" totalsRowShown="0">
+  <autoFilter ref="A1:G13"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Item #"/>
     <tableColumn id="2" name="Description"/>
@@ -413,24 +467,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" customWidth="1"/>
+    <col min="4" max="4" width="6.69921875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +506,12 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1">
+        <f>SUM(G2:G30)</f>
+        <v>41.27000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -476,7 +534,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -499,7 +557,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -520,6 +578,203 @@
       </c>
       <c r="G4">
         <v>4.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0.26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <f>D6*E6</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0.59</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:G13" si="0">D7*E7</f>
+        <v>5.8999999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0.92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>9.2000000000000011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0.3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>0.19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>0.32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>0.26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>0.441</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>4.41</v>
       </c>
     </row>
   </sheetData>
@@ -527,11 +782,19 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C10" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
+    <hyperlink ref="C12" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added components for blinker circuit
</commit_message>
<xml_diff>
--- a/Expenses/PCB connector Bill.xlsx
+++ b/Expenses/PCB connector Bill.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewazmy/Desktop/Supermileage ALL/Supermileage/trunk/Expenses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\SVN\trunk\Expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14556" tabRatio="311"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Item #</t>
   </si>
@@ -66,15 +66,60 @@
   </si>
   <si>
     <t>CAD</t>
+  </si>
+  <si>
+    <t>8-DIP Socket for 555</t>
+  </si>
+  <si>
+    <t>A08-LC-TT</t>
+  </si>
+  <si>
+    <t>555 Timer Circuit</t>
+  </si>
+  <si>
+    <t>LM555CN</t>
+  </si>
+  <si>
+    <t>5V Voltage Regulator</t>
+  </si>
+  <si>
+    <t>L7805ABD2T-TR</t>
+  </si>
+  <si>
+    <t>TMK316F106ZL-T</t>
+  </si>
+  <si>
+    <t>10uF Capacitor</t>
+  </si>
+  <si>
+    <t>10nF Capacitor</t>
+  </si>
+  <si>
+    <t>CC1206KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>1k Resistor</t>
+  </si>
+  <si>
+    <t>ERJ-14YJ102U</t>
+  </si>
+  <si>
+    <t>ERJ-14YJ223U</t>
+  </si>
+  <si>
+    <t>22k Resistor</t>
+  </si>
+  <si>
+    <t>50k Resistor</t>
+  </si>
+  <si>
+    <t>CRCW121049K9FKEA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -118,12 +163,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -135,13 +178,16 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0">
-  <autoFilter ref="A1:G4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G13" totalsRowShown="0">
+  <autoFilter ref="A1:G13"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Item #"/>
     <tableColumn id="2" name="Description"/>
@@ -418,24 +464,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" customWidth="1"/>
+    <col min="4" max="4" width="6.69921875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +503,12 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H1">
+        <f>SUM(G2:G30)</f>
+        <v>41.27000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,7 +531,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -504,7 +554,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -527,197 +577,216 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>0.26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <f>D5*E5</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>0.59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G12" si="0">D6*E6</f>
+        <v>5.8999999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0.92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>9.2000000000000011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>0.3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0.19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>0.32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>0.26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>0.441</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>4.41</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated billing information for harnesses
</commit_message>
<xml_diff>
--- a/Expenses/PCB connector Bill.xlsx
+++ b/Expenses/PCB connector Bill.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\SVN\trunk\Expenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewazmy/Desktop/Supermileage ALL/Supermileage/trunk/Expenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14556" tabRatio="311"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="311"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Item #</t>
   </si>
@@ -114,13 +114,100 @@
   </si>
   <si>
     <t>CRCW121049K9FKEA</t>
+  </si>
+  <si>
+    <t>Harness Size 23 Type 1</t>
+  </si>
+  <si>
+    <t>206838-1</t>
+  </si>
+  <si>
+    <t>Harness Size 23 Type 3</t>
+  </si>
+  <si>
+    <t>206137-1</t>
+  </si>
+  <si>
+    <t>Harness Size 17 Type 1</t>
+  </si>
+  <si>
+    <t>206036-1</t>
+  </si>
+  <si>
+    <t>Harness Size 13 Type 1</t>
+  </si>
+  <si>
+    <t>206705-1</t>
+  </si>
+  <si>
+    <t>Harness Size 11 Type 1</t>
+  </si>
+  <si>
+    <t>206061-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clamp Size 23 </t>
+  </si>
+  <si>
+    <t>206138-8</t>
+  </si>
+  <si>
+    <t>Clamp Size 17</t>
+  </si>
+  <si>
+    <t>206070-8</t>
+  </si>
+  <si>
+    <t>Clamp Size 13</t>
+  </si>
+  <si>
+    <t>206966-7</t>
+  </si>
+  <si>
+    <t>Clamp Size 11</t>
+  </si>
+  <si>
+    <t>1-206062-4</t>
+  </si>
+  <si>
+    <t>Plug Size 17</t>
+  </si>
+  <si>
+    <t>206037-1</t>
+  </si>
+  <si>
+    <t>Plug Size 13</t>
+  </si>
+  <si>
+    <t>206708-1</t>
+  </si>
+  <si>
+    <t>Plug Size 23</t>
+  </si>
+  <si>
+    <t>206837-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pins </t>
+  </si>
+  <si>
+    <t xml:space="preserve">66361-3 </t>
+  </si>
+  <si>
+    <t>Sockets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66360-3 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,16 +228,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FFBDD7EE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -158,15 +268,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -186,8 +332,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G13" totalsRowShown="0">
-  <autoFilter ref="A1:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G34" totalsRowShown="0">
+  <autoFilter ref="A1:G34"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Item #"/>
     <tableColumn id="2" name="Description"/>
@@ -464,21 +610,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="18.69921875" customWidth="1"/>
-    <col min="4" max="4" width="6.69921875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="11.19921875" customWidth="1"/>
-    <col min="7" max="7" width="12.19921875" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -505,7 +651,7 @@
       </c>
       <c r="H1">
         <f>SUM(G2:G30)</f>
-        <v>41.27000000000001</v>
+        <v>692.18000000000006</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -745,7 +891,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -767,6 +913,328 @@
       <c r="G12">
         <f t="shared" si="0"/>
         <v>4.41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>6.95</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>10.7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="10">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="7">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9">
+        <v>4.57</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="10">
+        <v>31.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3.84</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="6">
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="7">
+        <v>3</v>
+      </c>
+      <c r="E18" s="9">
+        <v>6.74</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="10">
+        <v>20.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="3">
+        <v>6</v>
+      </c>
+      <c r="E19" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="6">
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="7">
+        <v>7</v>
+      </c>
+      <c r="E20" s="9">
+        <v>6.99</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="10">
+        <v>48.93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>5.86</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6">
+        <v>11.72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="7">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9">
+        <v>7.06</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="10">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5">
+        <v>5.51</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="6">
+        <v>16.53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>8.92</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="10">
+        <v>17.84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="3">
+        <v>200</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.74</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="6">
+        <v>148.80000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="7">
+        <v>200</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1.08</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="10">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -782,11 +1250,25 @@
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
     <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made Changes, updated price and added rin rail stuff (Not including Sahil's stuff)
</commit_message>
<xml_diff>
--- a/Expenses/PCB connector Bill.xlsx
+++ b/Expenses/PCB connector Bill.xlsx
@@ -1,31 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewazmy/Desktop/Supermileage ALL/Supermileage/trunk/Expenses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\Documents\School Stuff\Supermileage\Schematics.git\trunk\Expenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="311"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14505" tabRatio="311"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Item #</t>
   </si>
@@ -48,24 +44,6 @@
     <t>Manufactur Part#</t>
   </si>
   <si>
-    <t>51216-0200</t>
-  </si>
-  <si>
-    <t>Receptacle Housing</t>
-  </si>
-  <si>
-    <t>Terminal Retainer</t>
-  </si>
-  <si>
-    <t>51217-0205</t>
-  </si>
-  <si>
-    <t>Vertical Header</t>
-  </si>
-  <si>
-    <t>55755-0219</t>
-  </si>
-  <si>
     <t>CAD</t>
   </si>
   <si>
@@ -199,6 +177,18 @@
   </si>
   <si>
     <t xml:space="preserve">66360-3 </t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Din Rail Terminal Block</t>
+  </si>
+  <si>
+    <t>Din Rail End Block</t>
+  </si>
+  <si>
+    <t>Din Rail Terminal Jumpers</t>
   </si>
 </sst>
 </file>
@@ -206,7 +196,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -410,12 +400,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -427,12 +416,17 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -446,16 +440,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G26" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G27" totalsRowCount="1">
   <autoFilter ref="A1:G26"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Item #"/>
+    <tableColumn id="1" name="Item #" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Manufactur Part#"/>
     <tableColumn id="4" name="Qty"/>
     <tableColumn id="5" name="Price/Unit"/>
     <tableColumn id="6" name="Currency"/>
-    <tableColumn id="7" name="Total(CAD)"/>
+    <tableColumn id="7" name="Total(CAD)" totalsRowFunction="sum" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -724,24 +718,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
+    <col min="7" max="7" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,89 +757,30 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1">
-        <f>SUM(G2:G22)</f>
-        <v>659.37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3">
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4">
-        <v>4.79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -854,44 +789,46 @@
         <v>6.95</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="6">
+        <v>7</v>
+      </c>
+      <c r="G5" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
         <v>13.9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>10.7</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="10">
+      <c r="F6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
         <v>21.4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3">
         <v>6</v>
@@ -900,44 +837,46 @@
         <v>4.5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="6">
+        <v>7</v>
+      </c>
+      <c r="G7" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="7">
-        <v>7</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8">
         <v>4.57</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="10">
-        <v>31.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="F8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>31.990000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3">
         <v>2</v>
@@ -946,243 +885,361 @@
         <v>3.84</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="6">
+        <v>7</v>
+      </c>
+      <c r="G9" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
         <v>7.68</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>6.74</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="10">
+      <c r="F10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
         <v>20.22</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3">
         <v>6</v>
       </c>
       <c r="E11" s="5">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="6">
-        <v>33.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="G11" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="7">
-        <v>7</v>
-      </c>
-      <c r="E12" s="9">
-        <v>6.99</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="10">
-        <v>48.93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="6">
+        <v>7</v>
+      </c>
+      <c r="E12" s="8">
+        <v>7.12</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>49.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3">
         <v>2</v>
       </c>
       <c r="E13" s="5">
-        <v>5.86</v>
+        <v>5.96</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="6">
-        <v>11.72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="G13" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>11.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6">
         <v>5</v>
       </c>
-      <c r="E14" s="9">
-        <v>7.06</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="10">
-        <v>35.299999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="E14" s="8">
+        <v>7.11</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>35.550000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3">
         <v>3</v>
       </c>
       <c r="E15" s="5">
-        <v>5.51</v>
+        <v>5.55</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="6">
-        <v>16.53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="G15" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>16.649999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="B16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="6">
         <v>2</v>
       </c>
-      <c r="E16" s="9">
-        <v>8.92</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="10">
-        <v>17.84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="E16" s="8">
+        <v>8.98</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>17.96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D17" s="3">
         <v>200</v>
       </c>
       <c r="E17" s="5">
-        <v>0.74</v>
+        <v>0.61350000000000005</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="6">
-        <v>148.80000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>122.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="B18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="6">
         <v>200</v>
       </c>
-      <c r="E18" s="9">
-        <v>1.08</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="10">
-        <v>216</v>
+      <c r="E18" s="8">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>107.80000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3031241</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>2.6880000000000002</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>53.760000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3022276</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>1.62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>9.7200000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3030161</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>18.580000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="9">
+        <f>Table1[[#This Row],[Price/Unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="21">
+        <f>SUBTOTAL(109,Table1[Total(CAD)])</f>
+        <v>600.87</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C8" r:id="rId1"/>
+    <hyperlink ref="C9" r:id="rId2"/>
+    <hyperlink ref="C10" r:id="rId3"/>
+    <hyperlink ref="C11" r:id="rId4"/>
+    <hyperlink ref="C12" r:id="rId5"/>
+    <hyperlink ref="C13" r:id="rId6"/>
+    <hyperlink ref="C14" r:id="rId7"/>
+    <hyperlink ref="C15" r:id="rId8"/>
+    <hyperlink ref="C16" r:id="rId9"/>
+    <hyperlink ref="C17" r:id="rId10"/>
+    <hyperlink ref="C18" r:id="rId11"/>
+    <hyperlink ref="C19" r:id="rId12" display="3037277"/>
+    <hyperlink ref="C20" r:id="rId13" display="30222776"/>
+    <hyperlink ref="C21" r:id="rId14" display="3030161"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId19"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1195,223 +1252,223 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21">
+    <row r="2" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="18">
+      <c r="B2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="17">
         <v>10</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="17">
         <v>0.26</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="20">
+      <c r="F2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="19">
         <f>D2*E2</f>
         <v>2.6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="14">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15">
+      <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="15">
+      <c r="C3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14">
         <v>0.59</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="17">
+      <c r="F3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="16">
         <f t="shared" ref="G3:G9" si="0">D3*E3</f>
         <v>5.8999999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="18">
+      <c r="B4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="17">
         <v>10</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>0.92</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="F4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="19">
         <f t="shared" si="0"/>
         <v>9.2000000000000011</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="21">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="14">
         <v>10</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>0.3</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="17">
+      <c r="F5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="18">
+      <c r="B6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="17">
         <v>10</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>0.19</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="20">
+      <c r="F6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="19">
         <f t="shared" si="0"/>
         <v>1.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="15">
+      <c r="B7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="14">
         <v>10</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>0.32</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="17">
+      <c r="F7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="16">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="21">
-        <v>7</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="18">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="17">
         <v>10</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <v>0.26</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="20">
+      <c r="F8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="19">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="14">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="15">
+      <c r="B9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="14">
         <v>10</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0.441</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="17">
+      <c r="F9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="16">
         <f t="shared" si="0"/>
         <v>4.41</v>
       </c>

</xml_diff>